<commit_message>
i add falsk code i will update everything, just testing selenium in falsk and every thing works good, but i need struct the code and add a better web files
</commit_message>
<xml_diff>
--- a/clear_tweets.xlsx
+++ b/clear_tweets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,6 @@
           <t>Tweets</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>sentiments</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -471,11 +466,6 @@
           <t>india israel tip shoe</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -493,11 +483,6 @@
           <t>peopl kashmir palestin look us want see unifi respons us human right democrat right rais voic everi forum former prime minist pakistan imran khan</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -515,11 +500,6 @@
           <t>break missil attack isra base northern occupi media sourc</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -537,11 +517,6 @@
           <t>isra forc arrest islam state oper west bank immin terror attack thwart</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -559,11 +534,6 @@
           <t>mute enjoy life pakistan think issu headach rais voic watch video say next target</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -581,11 +551,6 @@
           <t>colleg histori professor told palestin invent ident realli jordanian thing palestin wish could send book 4th shelf</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -603,11 +568,6 @@
           <t>peopl kashmir palestin look us want see unifi respons us human right democrat right rais voic everi forum former prime minist pakistan imran khan</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -623,11 +583,6 @@
       <c r="C9" t="inlineStr">
         <is>
           <t>wander sylvia import messag</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -643,11 +598,6 @@
           <t>195 countri state leader support think</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -665,11 +615,6 @@
           <t>unicef execut director declar situat gaza strip shock 13000 palestinian children die result attack regim</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -687,11 +632,6 @@
           <t>must watch video sign hour near</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -709,11 +649,6 @@
           <t>everi indian watch support israel</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -731,11 +666,6 @@
           <t>support ralli centr berlin express solidar palestinian</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -753,11 +683,6 @@
           <t>octob 7 never begin stori see isra treat palestinian women octob 7 invit femal fan freedom life world watch clip</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -775,11 +700,6 @@
           <t>martyr soleimani breath new life resist front open new path imam khamenei</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -797,11 +717,6 @@
           <t>stand iran</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -819,11 +734,6 @@
           <t>let us check road blocker whine whilst em remov hand contrapt will place unfortun look like handarm fine</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -841,11 +751,6 @@
           <t>kushner say american fund ethnic cleans build real estat american go bankrupt fund jewish supremaci white hous</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -863,11 +768,6 @@
           <t>– holi quran let peopl enmiti incit act otherwis justic alway nearer righteous 59</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -885,11 +785,6 @@
           <t>help sanaa sujood famili evacu palestin share donat gfm</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -907,11 +802,6 @@
           <t>pray stand palestin</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -929,11 +819,6 @@
           <t>everi decent human stand</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -951,11 +836,6 @@
           <t>video show moment driver stuck bridg confront group propalestinian demonstr san francisco today organ say protest part a15 global econom blockad solidar</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -973,11 +853,6 @@
           <t>go hell child killer</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -995,11 +870,6 @@
           <t>asylum migrat pact consolid encourag facilit wareh asylum seeker wareh peopl open air prison call decad wonder say share valu israel</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1017,11 +887,6 @@
           <t>conflict explain key moment shape histori constant war</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1039,11 +904,6 @@
           <t>iran put arm forc full high alert time iran would respond direct stand iran stand</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1061,11 +921,6 @@
           <t>break news israel send jordanian rambo attack iran thing progress</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1083,11 +938,6 @@
           <t>artist art martyr tehranimoghaddam</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1105,11 +955,6 @@
           <t>big rain loud storm hit uae make flood car stuck road betray look like</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1127,11 +972,6 @@
           <t>question support heart human butcher kid wrong genocid colonis ethnic cleans innoc peopl wrong steal land wrong ask question problem</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1149,11 +989,6 @@
           <t>assalamu alaikum 𝐒𝐮𝐛𝐚𝐡 𝐚𝐥 𝐤𝐡𝐞𝐢𝐫 end choos one among option let us know comment 1 two state solut 2the entir land given 3end</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1171,11 +1006,6 @@
           <t>like mosquito zionist suck blood countri regrett muslim govern help zionist regim amid conflict</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1193,11 +1023,6 @@
           <t>london solidar judaism zionism diametr oppos</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1215,11 +1040,6 @@
           <t>heartbroken palestin word express sorrow</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1237,11 +1057,6 @@
           <t>know know remind</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1259,11 +1074,6 @@
           <t>right iranian gather squar</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1281,11 +1091,6 @@
           <t>palestin free karwa rahi thi paw paw ab 16 charg face kar rahi hu previous post fk modi facebook page end get fuke court</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1303,11 +1108,6 @@
           <t>south africa spinner tabraiz shamsi announc support palestin massiv respect</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1325,11 +1125,6 @@
           <t>alway</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1347,11 +1142,6 @@
           <t>urg western media outlet abandon frame activ shield israel respons crime peopl util frame recogn bind natur intern law concern western media…</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1369,11 +1159,6 @@
           <t>hand guy ask whether muslim say muslim indian hindu palestinian person even forc eat cow beef watch video shubham describ incid</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1391,11 +1176,6 @@
           <t>despit kill destruct displac ethnic cleans racism occup return father grandfath home farm oliv tree land sign never forget never forgiv</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1413,11 +1193,6 @@
           <t>new york hillard newspap 100 year ago front page date 12111917 day occup headlin bold britain save 673 year muslim rule</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1435,11 +1210,6 @@
           <t>ishowspe say “bye bye israel”</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1457,11 +1227,6 @@
           <t>– outrag parliament mani countri includ canada word continu spread innoc palestinian civilian shot kill wait humanitarian aid</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1479,11 +1244,6 @@
           <t>protest profanityladen chant middl finger act nonviol defianc polic apr 16 2024</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1501,11 +1261,6 @@
           <t>like mosquito zionist suck blood countri</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1523,11 +1278,6 @@
           <t>alert east news gather attack town</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1545,11 +1295,6 @@
           <t>easi fearmong bomb kid impun outrag 100k hurt illeg blockad though weapon rain west stay mute tax fund apartheid yet refuge flee “threats” hypocrit ignor israels…</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1567,11 +1312,6 @@
           <t>river sea free</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1589,11 +1329,6 @@
           <t>mother wit murder children agre</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1611,11 +1346,6 @@
           <t>good news gotten basic everyth set chariti stream event inde happen june 10th june 17th make sure help</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1633,11 +1363,6 @@
           <t>apost one protect zionist regim repres muslim inshaallah day come muslim fight overthrow murtaddeen</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1655,11 +1380,6 @@
           <t>retali zionist attack iranian consul scene occupi</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1677,11 +1397,6 @@
           <t>attack extrem danger use idiot lefti muslim march celebr iran attack back mysoginist murder islam revolutionari regim ban protest</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1699,11 +1414,6 @@
           <t>power act solidar</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1721,11 +1431,6 @@
           <t>syria real test muslim</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1743,11 +1448,6 @@
           <t>west bank attack arm isra settler burn entir palestinian villag ground</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1765,11 +1465,6 @@
           <t>austrian women take palestin support poster india</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1787,11 +1482,6 @@
           <t>univers california faculti justic open letter dean chemerinski full text avail</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1809,11 +1499,6 @@
           <t>dozen fanat isra settler attack palestinian resid almughay villag ramallah occupi west bank</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1831,11 +1516,6 @@
           <t>driver get upset protest block golden gate bridg polic respond noth stop crimin obstruct movement crime ca road</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1853,11 +1533,6 @@
           <t>displac child gaza sing injur brother</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1875,11 +1550,6 @@
           <t>hear geezer anoth nicknam genocid joe pass opportun make anoth gif use standard compon show support palestinian gif download</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1897,11 +1567,6 @@
           <t>pakistani littl girl midhet zehra donat eid gift money children real</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1919,11 +1584,6 @@
           <t>know king abdullah train help destitut</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1941,11 +1601,6 @@
           <t>saturday london march assembl 12 noon russel squar – march parliament squar support isra state never precari letup drive must keep push making…</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1963,11 +1618,6 @@
           <t>wednesday resist target newli establish headquart militari reconnaiss compani arab alaramsheh mark first kind term casualti northern occupi sinc begin israel war on…</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1985,11 +1635,6 @@
           <t>book recommend read</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2007,11 +1652,6 @@
           <t>bigotri censorship appal countri pioneer free speech let univers silenc voic student sicken condemn cancel valedictorian speech</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2029,11 +1669,6 @@
           <t>shout kashmiri brother sister oppress around globe</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2051,11 +1686,6 @@
           <t>friend due polici content account close campaign save famili withdrew fund set gofundm cover remain expens evacu famili pleas share donat</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2073,11 +1703,6 @@
           <t>precious weapon contract friend israel cheer war crime go unpunish</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2095,11 +1720,6 @@
           <t>retweet support</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2117,11 +1737,6 @@
           <t>protest use colour languag accus polic damag vehicl park outsid scrap yardbodi shop apr 16 2024</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2139,11 +1754,6 @@
           <t>today latest news kuwait warn america use land iran pray palestin iran</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2161,11 +1771,6 @@
           <t>rare footag palestinian address british govern 1936</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2183,11 +1788,6 @@
           <t>wang yi china support becom full member state unit nation</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>positive</t>
-        </is>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2205,11 +1805,6 @@
           <t>polic ask protest move back railway track shove match tri hold line</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2227,11 +1822,6 @@
           <t>russian presid putin say palestin histor belong palestinian</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2249,11 +1839,6 @@
           <t>ask other continu voic peopl go genocid likepeopl</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>negative</t>
-        </is>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2271,11 +1856,6 @@
           <t>unlik polit leader peopl speak atroc carri protest airport today civilian airport neutral countri abus militari two decad</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2293,11 +1873,6 @@
           <t>current visual isra shawi shomron town sebastia palestin</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2315,11 +1890,6 @@
           <t>us defens secretari austin said evid israel commit genocid gaza fact lie cannot cover truth israel commit genocid gaza</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2337,11 +1907,6 @@
           <t>western media use word dehuman palestinian</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2359,11 +1924,6 @@
           <t>protest yell polic offic switch bodi cam hit videograph record public</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>neutral</t>
-        </is>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2379,11 +1939,6 @@
       <c r="C89" t="inlineStr">
         <is>
           <t>bodi free children gaza free children innoc ceasefir save children side genocid</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>positive</t>
         </is>
       </c>
     </row>

</xml_diff>